<commit_message>
add iterative speed finder for trajectories. add basic client-side settings (non-persistent).
</commit_message>
<xml_diff>
--- a/AncientWarfare/src/shadowmage/ancient_warfare/resources/45deg angle vel calc.xlsx
+++ b/AncientWarfare/src/shadowmage/ancient_warfare/resources/45deg angle vel calc.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19035" windowHeight="11505"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19035" windowHeight="11505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>g</t>
   </si>
@@ -41,6 +43,30 @@
   </si>
   <si>
     <t>top</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>yhit=</t>
+  </si>
+  <si>
+    <t>xtan(a)</t>
+  </si>
+  <si>
+    <t>2u^2</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>sqrt</t>
   </si>
 </sst>
 </file>
@@ -375,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -394,7 +420,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -402,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-2.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -425,7 +451,7 @@
       </c>
       <c r="F7">
         <f>B2*TAN(B4)</f>
-        <v>9.7186511432631697</v>
+        <v>161.97751905438616</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -434,7 +460,7 @@
       </c>
       <c r="B8">
         <f>B3</f>
-        <v>-2.63</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -444,7 +470,7 @@
       </c>
       <c r="F8">
         <f>B1*B2*B2</f>
-        <v>353.15999999999997</v>
+        <v>98100</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -462,29 +488,252 @@
       </c>
       <c r="D14">
         <f>B1*2*B2*B2</f>
-        <v>706.31999999999994</v>
+        <v>196200</v>
       </c>
       <c r="E14">
-        <f>D14/2</f>
-        <v>353.15999999999997</v>
+        <f>F8</f>
+        <v>98100</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="G15">
         <f>B2-B3</f>
-        <v>8.629999999999999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="6:6">
       <c r="F17">
         <f>E14/G15</f>
-        <v>40.92236384704519</v>
+        <v>981</v>
       </c>
     </row>
     <row r="18" spans="6:6">
       <c r="F18">
         <f>SQRT(F17)</f>
-        <v>6.397058999809615</v>
+        <v>31.32091952673165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <f>B2*TAN(B4)</f>
+        <v>48.593255716315845</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <f>2*POWER(B5,2)</f>
+        <v>2178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <f>B1 * POWER(B2,2)</f>
+        <v>9000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <f>POWER(COS(B4),2)</f>
+        <v>0.27596319193541496</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <f>C10 - (C11 / F10*F11)</f>
+        <v>47.452911947987687</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>33.014282000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <f>B5*B5</f>
+        <v>1089.9428159755241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f>B5*B5*B5*B5</f>
+        <v>1187975.3420966552</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <f>B2*B2</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <f>SQRT(B10-B1*(B1*B11+2*B3*B9))</f>
+        <v>108.47839232887438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <f>B9+B12</f>
+        <v>1198.4212083043985</v>
+      </c>
+      <c r="B14">
+        <f>A14/ (B1*B2)</f>
+        <v>1.2216322204937804</v>
+      </c>
+      <c r="C14">
+        <f>ATAN(B14)</f>
+        <v>0.88483016261103575</v>
+      </c>
+      <c r="D14">
+        <f>DEGREES(C14)</f>
+        <v>50.697033903486684</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <f>B9-B12</f>
+        <v>981.46442364664972</v>
+      </c>
+      <c r="B15">
+        <f>A15/(B1*B2)</f>
+        <v>1.0004734186000508</v>
+      </c>
+      <c r="C15">
+        <f>ATAN(B15)</f>
+        <v>0.78563481667502311</v>
+      </c>
+      <c r="D15">
+        <f>DEGREES(C15)</f>
+        <v>45.013559234012973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>